<commit_message>
updated readme.md with test clasess
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata1.xlsx
+++ b/src/main/resources/testdata1.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA_projects\SeleniumTraining\SeleniumFramework\src\main\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17295" windowHeight="7275"/>
   </bookViews>
   <sheets>
     <sheet name="testdata" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -406,10 +402,11 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>